<commit_message>
Updated User DB with encoded data.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Users.xlsx
+++ b/src/test/resources/data/Users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MTRPE\OneDrive\Desktop\JAVA Projects\financialPeaceUniversity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MTRPE\OneDrive\Desktop\JAVA Projects\financialPeaceUniversity\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF14FF63-98C1-4FAA-A73E-77092180BD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476475C5-0769-4902-A250-8F490AFCBBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AFFDEE9F-3302-4BE4-A11D-FD1232A928A6}"/>
+    <workbookView xWindow="10650" yWindow="6345" windowWidth="17055" windowHeight="11295" xr2:uid="{AFFDEE9F-3302-4BE4-A11D-FD1232A928A6}"/>
   </bookViews>
   <sheets>
     <sheet name="existingUserInfo" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>userName</t>
   </si>
@@ -47,13 +47,7 @@
     <t>userPassword</t>
   </si>
   <si>
-    <t>Goce Trpevski</t>
-  </si>
-  <si>
-    <t>gocesdet@gmail.com</t>
-  </si>
-  <si>
-    <t>UserUser@123</t>
+    <t>Z29jZXNkZXRAZ21haWwuY29t</t>
   </si>
 </sst>
 </file>
@@ -89,9 +83,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,14 +402,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -434,11 +425,11 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>